<commit_message>
Fittings completed, constants found
</commit_message>
<xml_diff>
--- a/Post analysis/Excel work/Regression fittings constants.xlsx
+++ b/Post analysis/Excel work/Regression fittings constants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>a</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>cycle</t>
+  </si>
+  <si>
+    <t>Time (min)</t>
   </si>
 </sst>
 </file>
@@ -273,25 +279,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -307,6 +298,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -423,12 +429,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="40883712"/>
-        <c:axId val="40882176"/>
+        <c:axId val="111549056"/>
+        <c:axId val="111672704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40883712"/>
+        <c:axId val="111549056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,13 +463,13 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40882176"/>
+        <c:crossAx val="111672704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40882176"/>
+        <c:axId val="111672704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -492,7 +497,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40883712"/>
+        <c:crossAx val="111549056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -505,7 +510,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -515,16 +520,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -831,66 +836,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J10"/>
+  <dimension ref="B1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="6" width="9.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:10">
-      <c r="B2" s="5"/>
-      <c r="C2" s="9" t="s">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:18">
+      <c r="B2" s="15"/>
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="13"/>
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="13"/>
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="11" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="6"/>
-      <c r="C3" s="14" t="s">
+      <c r="J2" s="13"/>
+      <c r="N2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="16"/>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="12" t="s">
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1789.67</v>
+      </c>
+      <c r="P3">
+        <v>954.88</v>
+      </c>
+      <c r="Q3">
+        <v>0.93589999999999995</v>
+      </c>
+      <c r="R3">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2">
@@ -911,15 +947,30 @@
       <c r="H4" s="1">
         <v>1.17</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>63.8</v>
       </c>
       <c r="J4" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="12" t="s">
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>1818.53</v>
+      </c>
+      <c r="P4">
+        <v>968.29</v>
+      </c>
+      <c r="Q4">
+        <v>0.94359999999999999</v>
+      </c>
+      <c r="R4">
+        <v>19.579999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2">
@@ -940,15 +991,27 @@
       <c r="H5" s="1">
         <v>2.1</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>45.45</v>
       </c>
       <c r="J5" s="1">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B6" s="13" t="s">
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>1751.82</v>
+      </c>
+      <c r="P5">
+        <v>943.04</v>
+      </c>
+      <c r="Q5">
+        <v>0.94369999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" ht="15.75" thickBot="1">
+      <c r="B6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3">
@@ -969,14 +1032,68 @@
       <c r="H6" s="4">
         <v>1E-3</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>0.95579999999999998</v>
       </c>
       <c r="J6" s="4">
         <v>1.1999999999999999E-3</v>
       </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>1690.67</v>
+      </c>
+      <c r="P6">
+        <v>910.02</v>
+      </c>
+      <c r="Q6">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>1593.19</v>
+      </c>
+      <c r="P7">
+        <v>890.65</v>
+      </c>
+      <c r="Q7">
+        <v>0.94159999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8">
+        <v>1526.54</v>
+      </c>
+      <c r="P8">
+        <v>856.78</v>
+      </c>
+      <c r="Q8">
+        <v>0.94259999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="N9">
+        <v>7</v>
+      </c>
+      <c r="O9">
+        <v>1464.97</v>
+      </c>
+      <c r="P9">
+        <v>807.53</v>
+      </c>
+      <c r="Q9">
+        <v>0.94450000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
       <c r="C10">
         <f>(C6+E6+G6+I6)/4</f>
         <v>0.95317499999999988</v>
@@ -984,6 +1101,382 @@
       <c r="D10">
         <f>1/4*SQRT(D6^2+F6^2+H6^2+J6^2)</f>
         <v>8.1124903697939752E-4</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>1399.08</v>
+      </c>
+      <c r="P10">
+        <v>777.34</v>
+      </c>
+      <c r="Q10">
+        <v>0.94579999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18">
+      <c r="N11">
+        <v>9</v>
+      </c>
+      <c r="O11">
+        <v>1351.82</v>
+      </c>
+      <c r="P11">
+        <v>762.14</v>
+      </c>
+      <c r="Q11">
+        <v>0.95030000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18">
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>1315.76</v>
+      </c>
+      <c r="P12">
+        <v>753.69</v>
+      </c>
+      <c r="Q12">
+        <v>0.95630000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="N13">
+        <v>11</v>
+      </c>
+      <c r="O13">
+        <v>1265.31</v>
+      </c>
+      <c r="P13">
+        <v>768.72</v>
+      </c>
+      <c r="Q13">
+        <v>0.96020000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="N14">
+        <v>12</v>
+      </c>
+      <c r="O14">
+        <v>1183.74</v>
+      </c>
+      <c r="P14">
+        <v>728.74</v>
+      </c>
+      <c r="Q14">
+        <v>0.96040000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="N15">
+        <v>13</v>
+      </c>
+      <c r="O15">
+        <v>1016.2</v>
+      </c>
+      <c r="P15">
+        <v>632.07000000000005</v>
+      </c>
+      <c r="Q15">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18">
+      <c r="N16">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <v>879.69</v>
+      </c>
+      <c r="P16">
+        <v>531.30999999999995</v>
+      </c>
+      <c r="Q16">
+        <v>0.95840000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="14:17">
+      <c r="N17">
+        <v>15</v>
+      </c>
+      <c r="O17">
+        <v>763.3</v>
+      </c>
+      <c r="P17">
+        <v>481.85</v>
+      </c>
+      <c r="Q17">
+        <v>0.95669999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="14:17">
+      <c r="N18">
+        <v>16</v>
+      </c>
+      <c r="O18">
+        <v>663.5</v>
+      </c>
+      <c r="P18">
+        <v>414.35</v>
+      </c>
+      <c r="Q18">
+        <v>0.95669999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="14:17">
+      <c r="N19">
+        <v>17</v>
+      </c>
+      <c r="O19">
+        <v>588.04</v>
+      </c>
+      <c r="P19">
+        <v>361.68</v>
+      </c>
+      <c r="Q19">
+        <v>0.95550000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="14:17">
+      <c r="N20">
+        <v>18</v>
+      </c>
+      <c r="O20">
+        <v>536.29</v>
+      </c>
+      <c r="P20">
+        <v>338.14</v>
+      </c>
+      <c r="Q20">
+        <v>0.95830000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="14:17">
+      <c r="N21">
+        <v>19</v>
+      </c>
+      <c r="O21">
+        <v>473.29</v>
+      </c>
+      <c r="P21">
+        <v>311.45</v>
+      </c>
+      <c r="Q21">
+        <v>0.95340000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="14:17">
+      <c r="N22">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <v>421.97</v>
+      </c>
+      <c r="P22">
+        <v>270.05</v>
+      </c>
+      <c r="Q22">
+        <v>0.95289999999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="14:17">
+      <c r="N23">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <v>372.53</v>
+      </c>
+      <c r="P23">
+        <v>239.69</v>
+      </c>
+      <c r="Q23">
+        <v>0.95169999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="14:17">
+      <c r="N24">
+        <v>22</v>
+      </c>
+      <c r="O24">
+        <v>338.59</v>
+      </c>
+      <c r="P24">
+        <v>221.46</v>
+      </c>
+      <c r="Q24">
+        <v>0.95620000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="14:17">
+      <c r="N25">
+        <v>23</v>
+      </c>
+      <c r="O25">
+        <v>297.88</v>
+      </c>
+      <c r="P25">
+        <v>199.13</v>
+      </c>
+      <c r="Q25">
+        <v>0.95330000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="14:17">
+      <c r="N26">
+        <v>24</v>
+      </c>
+      <c r="O26">
+        <v>268.05</v>
+      </c>
+      <c r="P26">
+        <v>178.5</v>
+      </c>
+      <c r="Q26">
+        <v>0.9546</v>
+      </c>
+    </row>
+    <row r="27" spans="14:17">
+      <c r="N27">
+        <v>25</v>
+      </c>
+      <c r="O27">
+        <v>229.11</v>
+      </c>
+      <c r="P27">
+        <v>154.25</v>
+      </c>
+      <c r="Q27">
+        <v>0.94699999999999995</v>
+      </c>
+    </row>
+    <row r="28" spans="14:17">
+      <c r="N28">
+        <v>26</v>
+      </c>
+      <c r="O28">
+        <v>201.74</v>
+      </c>
+      <c r="P28">
+        <v>137.22999999999999</v>
+      </c>
+      <c r="Q28">
+        <v>0.95020000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="14:17">
+      <c r="N29">
+        <v>27</v>
+      </c>
+      <c r="O29">
+        <v>176.22</v>
+      </c>
+      <c r="P29">
+        <v>121.64</v>
+      </c>
+      <c r="Q29">
+        <v>0.94710000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="14:17">
+      <c r="N30">
+        <v>28</v>
+      </c>
+      <c r="O30">
+        <v>147.13</v>
+      </c>
+      <c r="P30">
+        <v>97.91</v>
+      </c>
+      <c r="Q30">
+        <v>0.94699999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="14:17">
+      <c r="N31">
+        <v>29</v>
+      </c>
+      <c r="O31">
+        <v>130.66999999999999</v>
+      </c>
+      <c r="P31">
+        <v>90.45</v>
+      </c>
+      <c r="Q31">
+        <v>0.95199999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="14:17">
+      <c r="N32">
+        <v>30</v>
+      </c>
+      <c r="O32">
+        <v>111.04</v>
+      </c>
+      <c r="P32">
+        <v>78.069999999999993</v>
+      </c>
+      <c r="Q32">
+        <v>0.95009999999999994</v>
+      </c>
+    </row>
+    <row r="33" spans="14:17">
+      <c r="N33">
+        <v>31</v>
+      </c>
+      <c r="O33">
+        <v>91.84</v>
+      </c>
+      <c r="P33">
+        <v>63.34</v>
+      </c>
+      <c r="Q33">
+        <v>0.95409999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="14:17">
+      <c r="N34">
+        <v>32</v>
+      </c>
+      <c r="O34">
+        <v>78.45</v>
+      </c>
+      <c r="P34">
+        <v>53.77</v>
+      </c>
+      <c r="Q34">
+        <v>0.9556</v>
+      </c>
+    </row>
+    <row r="35" spans="14:17">
+      <c r="N35">
+        <v>33</v>
+      </c>
+      <c r="O35">
+        <v>63.65</v>
+      </c>
+      <c r="P35">
+        <v>45.55</v>
+      </c>
+      <c r="Q35">
+        <v>0.95520000000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="14:17">
+      <c r="N36">
+        <v>34</v>
+      </c>
+      <c r="O36">
+        <v>54.69</v>
+      </c>
+      <c r="P36">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="Q36">
+        <v>0.95740000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding the origin data analysis work and graphs
</commit_message>
<xml_diff>
--- a/Post analysis/Excel work/Regression fittings constants.xlsx
+++ b/Post analysis/Excel work/Regression fittings constants.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>a</t>
   </si>
@@ -98,6 +98,9 @@
   <si>
     <t>1-b/a</t>
   </si>
+  <si>
+    <t>Final pressure (mbar)</t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -408,11 +411,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,14 +496,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -471,21 +509,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -510,6 +533,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -544,6 +585,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -623,11 +665,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="110487040"/>
-        <c:axId val="110567424"/>
+        <c:axId val="119928320"/>
+        <c:axId val="119746560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="110487040"/>
+        <c:axId val="119928320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -653,16 +695,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110567424"/>
+        <c:crossAx val="119746560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="110567424"/>
+        <c:axId val="119746560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -685,23 +728,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110487040"/>
+        <c:crossAx val="119928320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1027,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:Z41"/>
+  <dimension ref="B1:AA41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="T4" activeCellId="1" sqref="O4:O35 T4:T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1040,78 +1085,82 @@
     <col min="17" max="17" width="13.28515625" style="12" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="20" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:26" ht="15.75" thickBot="1">
-      <c r="N2" s="37" t="s">
+    <row r="1" spans="2:27" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:27" ht="15.75" thickBot="1">
+      <c r="N2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="P2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="Q2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="33" t="s">
+      <c r="T2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="35" t="s">
+      <c r="U2" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B3" s="31"/>
-      <c r="C3" s="28" t="s">
+    <row r="3" spans="2:27" ht="15.75" thickBot="1">
+      <c r="B3" s="37"/>
+      <c r="C3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="35"/>
+      <c r="E3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="28" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="40"/>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="36"/>
-      <c r="V3" t="s">
+      <c r="J3" s="35"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="29"/>
+      <c r="W3" t="s">
         <v>23</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>24</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>25</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:26">
-      <c r="B4" s="32"/>
+    <row r="4" spans="2:27">
+      <c r="B4" s="38"/>
       <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
@@ -1136,52 +1185,55 @@
       <c r="J4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="21">
         <v>1</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="22">
         <v>1751.82</v>
       </c>
-      <c r="P4" s="24">
+      <c r="P4" s="22">
         <v>943.04</v>
       </c>
-      <c r="Q4" s="25">
+      <c r="Q4" s="23">
         <v>0.94369999999999998</v>
       </c>
-      <c r="R4" s="26">
+      <c r="R4" s="24">
         <v>21.083983333333332</v>
       </c>
-      <c r="S4" s="24">
+      <c r="S4" s="22">
         <v>5386</v>
       </c>
-      <c r="T4" s="24">
-        <v>464.9</v>
-      </c>
-      <c r="U4" s="27">
-        <f t="shared" ref="U4:U35" si="0">O4-T4</f>
-        <v>1286.92</v>
-      </c>
-      <c r="V4">
+      <c r="T4" s="22">
+        <v>662.2</v>
+      </c>
+      <c r="U4" s="39">
+        <v>660.2</v>
+      </c>
+      <c r="V4" s="25">
+        <f>O4-T4</f>
+        <v>1089.6199999999999</v>
+      </c>
+      <c r="W4">
         <f>P4/O4</f>
         <v>0.5383201470470711</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>0.5383201470470711</v>
       </c>
-      <c r="X4">
-        <f>O4*(1-W4)</f>
-        <v>808.77999999999986</v>
-      </c>
       <c r="Y4">
+        <f>O4-P4</f>
+        <v>808.78</v>
+      </c>
+      <c r="Z4">
         <f>T4/O4</f>
-        <v>0.26538114646481942</v>
-      </c>
-      <c r="Z4">
-        <f>1-V4</f>
+        <v>0.37800687285223372</v>
+      </c>
+      <c r="AA4">
+        <f>1-W4</f>
         <v>0.4616798529529289</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
+    <row r="5" spans="2:27">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
@@ -1228,33 +1280,36 @@
         <v>5818</v>
       </c>
       <c r="T5" s="13">
-        <v>436.1</v>
-      </c>
-      <c r="U5" s="17">
-        <f t="shared" si="0"/>
-        <v>1254.5700000000002</v>
-      </c>
-      <c r="V5">
-        <f t="shared" ref="V5:V35" si="1">P5/O5</f>
+        <v>635.20000000000005</v>
+      </c>
+      <c r="U5" s="40">
+        <v>631</v>
+      </c>
+      <c r="V5" s="25">
+        <f t="shared" ref="V5:V35" si="0">O5-T5</f>
+        <v>1055.47</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W35" si="1">P5/O5</f>
         <v>0.53825997977133322</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>0.53825997977133322</v>
       </c>
-      <c r="X5">
-        <f t="shared" ref="X5:X35" si="2">O5*(1-W5)</f>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y35" si="2">O5-P5</f>
         <v>780.65000000000009</v>
       </c>
-      <c r="Y5">
-        <f t="shared" ref="Y5:Y35" si="3">T5/O5</f>
-        <v>0.25794507502942621</v>
-      </c>
       <c r="Z5">
-        <f t="shared" ref="Z5:Z35" si="4">1-V5</f>
+        <f t="shared" ref="Z5:Z35" si="3">T5/O5</f>
+        <v>0.37570903842855202</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA35" si="4">1-W5</f>
         <v>0.46174002022866678</v>
       </c>
     </row>
-    <row r="6" spans="2:26">
+    <row r="6" spans="2:27">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1301,33 +1356,36 @@
         <v>6257</v>
       </c>
       <c r="T6" s="13">
-        <v>411.3</v>
-      </c>
-      <c r="U6" s="17">
+        <v>602</v>
+      </c>
+      <c r="U6" s="40">
+        <v>598.9</v>
+      </c>
+      <c r="V6" s="25">
         <f t="shared" si="0"/>
-        <v>1181.8900000000001</v>
-      </c>
-      <c r="V6">
+        <v>991.19</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="1"/>
         <v>0.5590356454660147</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>0.5590356454660147</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <f t="shared" si="2"/>
         <v>702.54000000000008</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <f t="shared" si="3"/>
-        <v>0.25816129902899215</v>
-      </c>
-      <c r="Z6">
+        <v>0.3778582592157872</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="4"/>
         <v>0.4409643545339853</v>
       </c>
     </row>
-    <row r="7" spans="2:26" ht="15.75" thickBot="1">
+    <row r="7" spans="2:27" ht="15.75" thickBot="1">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -1374,33 +1432,36 @@
         <v>6698</v>
       </c>
       <c r="T7" s="13">
-        <v>389.2</v>
-      </c>
-      <c r="U7" s="17">
+        <v>570.79999999999995</v>
+      </c>
+      <c r="U7" s="40">
+        <v>564</v>
+      </c>
+      <c r="V7" s="25">
         <f t="shared" si="0"/>
-        <v>1137.3399999999999</v>
-      </c>
-      <c r="V7">
+        <v>955.74</v>
+      </c>
+      <c r="W7">
         <f t="shared" si="1"/>
         <v>0.56125617409304707</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <v>0.56125617409304707</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <f t="shared" si="2"/>
-        <v>669.75999999999988</v>
-      </c>
-      <c r="Y7">
+        <v>669.76</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="3"/>
-        <v>0.25495565134225112</v>
-      </c>
-      <c r="Z7">
+        <v>0.37391748660369201</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="4"/>
         <v>0.43874382590695293</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:27">
       <c r="N8" s="16">
         <v>5</v>
       </c>
@@ -1420,33 +1481,36 @@
         <v>7128</v>
       </c>
       <c r="T8" s="13">
-        <v>366.1</v>
-      </c>
-      <c r="U8" s="17">
+        <v>538.79999999999995</v>
+      </c>
+      <c r="U8" s="40">
+        <v>532</v>
+      </c>
+      <c r="V8" s="25">
         <f t="shared" si="0"/>
-        <v>1098.8699999999999</v>
-      </c>
-      <c r="V8">
+        <v>926.17000000000007</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="1"/>
         <v>0.55122630497552849</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>0.55122630497552849</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f t="shared" si="2"/>
         <v>657.44</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <f t="shared" si="3"/>
-        <v>0.2499027283835164</v>
-      </c>
-      <c r="Z8">
+        <v>0.36778910148330679</v>
+      </c>
+      <c r="AA8">
         <f t="shared" si="4"/>
         <v>0.44877369502447151</v>
       </c>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:27">
       <c r="N9" s="16">
         <v>6</v>
       </c>
@@ -1466,33 +1530,36 @@
         <v>7542</v>
       </c>
       <c r="T9" s="13">
-        <v>341.2</v>
-      </c>
-      <c r="U9" s="17">
+        <v>507.1</v>
+      </c>
+      <c r="U9" s="40">
+        <v>500.6</v>
+      </c>
+      <c r="V9" s="25">
         <f t="shared" si="0"/>
-        <v>1057.8799999999999</v>
-      </c>
-      <c r="V9">
+        <v>891.9799999999999</v>
+      </c>
+      <c r="W9">
         <f t="shared" si="1"/>
         <v>0.55560797095234016</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>0.55560797095234016</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <f t="shared" si="2"/>
         <v>621.7399999999999</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <f t="shared" si="3"/>
-        <v>0.2438745461303142</v>
-      </c>
-      <c r="Z9">
+        <v>0.36245246876518861</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="4"/>
         <v>0.44439202904765984</v>
       </c>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:27">
       <c r="N10" s="16">
         <v>7</v>
       </c>
@@ -1512,33 +1579,36 @@
         <v>7995</v>
       </c>
       <c r="T10" s="13">
-        <v>315.5</v>
-      </c>
-      <c r="U10" s="17">
+        <v>472.9</v>
+      </c>
+      <c r="U10" s="40">
+        <v>463.5</v>
+      </c>
+      <c r="V10" s="25">
         <f t="shared" si="0"/>
-        <v>1036.32</v>
-      </c>
-      <c r="V10">
+        <v>878.92</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="1"/>
         <v>0.56378807829444755</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>0.56378807829444755</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <f t="shared" si="2"/>
-        <v>589.67999999999984</v>
-      </c>
-      <c r="Y10">
+        <v>589.67999999999995</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="3"/>
-        <v>0.23338906067375836</v>
-      </c>
-      <c r="Z10">
+        <v>0.34982468080069834</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="4"/>
         <v>0.43621192170555245</v>
       </c>
     </row>
-    <row r="11" spans="2:26">
+    <row r="11" spans="2:27">
       <c r="C11">
         <f>(C7+E7+G7+I7)/4</f>
         <v>0.95317499999999988</v>
@@ -1566,33 +1636,36 @@
         <v>8531</v>
       </c>
       <c r="T11" s="13">
-        <v>287.8</v>
-      </c>
-      <c r="U11" s="17">
+        <v>438.4</v>
+      </c>
+      <c r="U11" s="40">
+        <v>425.6</v>
+      </c>
+      <c r="V11" s="25">
         <f t="shared" si="0"/>
-        <v>1027.96</v>
-      </c>
-      <c r="V11">
+        <v>877.36</v>
+      </c>
+      <c r="W11">
         <f t="shared" si="1"/>
         <v>0.57281723110597682</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>0.57281723110597682</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f t="shared" si="2"/>
         <v>562.06999999999994</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <f t="shared" si="3"/>
-        <v>0.21873289961695144</v>
-      </c>
-      <c r="Z11">
+        <v>0.33319146348878215</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="4"/>
         <v>0.42718276889402318</v>
       </c>
     </row>
-    <row r="12" spans="2:26">
+    <row r="12" spans="2:27">
       <c r="N12" s="16">
         <v>9</v>
       </c>
@@ -1612,33 +1685,36 @@
         <v>9149</v>
       </c>
       <c r="T12" s="13">
-        <v>260.10000000000002</v>
-      </c>
-      <c r="U12" s="17">
+        <v>406.4</v>
+      </c>
+      <c r="U12" s="40">
+        <v>391.2</v>
+      </c>
+      <c r="V12" s="25">
         <f t="shared" si="0"/>
-        <v>1005.2099999999999</v>
-      </c>
-      <c r="V12">
+        <v>858.91</v>
+      </c>
+      <c r="W12">
         <f t="shared" si="1"/>
         <v>0.6075349123930105</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>0.6075349123930105</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <f t="shared" si="2"/>
-        <v>496.58999999999986</v>
-      </c>
-      <c r="Y12">
+        <v>496.58999999999992</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="3"/>
-        <v>0.20556227327690449</v>
-      </c>
-      <c r="Z12">
+        <v>0.32118611249417139</v>
+      </c>
+      <c r="AA12">
         <f t="shared" si="4"/>
         <v>0.3924650876069895</v>
       </c>
     </row>
-    <row r="13" spans="2:26">
+    <row r="13" spans="2:27">
       <c r="N13" s="16">
         <v>10</v>
       </c>
@@ -1658,33 +1734,36 @@
         <v>9846</v>
       </c>
       <c r="T13" s="13">
-        <v>235.3</v>
-      </c>
-      <c r="U13" s="17">
+        <v>373.7</v>
+      </c>
+      <c r="U13" s="40">
+        <v>336.6</v>
+      </c>
+      <c r="V13" s="25">
         <f t="shared" si="0"/>
-        <v>948.44</v>
-      </c>
-      <c r="V13">
+        <v>810.04</v>
+      </c>
+      <c r="W13">
         <f t="shared" si="1"/>
         <v>0.61562505279875646</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>0.61562505279875646</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <f t="shared" si="2"/>
-        <v>455.00000000000006</v>
-      </c>
-      <c r="Y13">
+        <v>455</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="3"/>
-        <v>0.19877675840978595</v>
-      </c>
-      <c r="Z13">
+        <v>0.31569432476726306</v>
+      </c>
+      <c r="AA13">
         <f t="shared" si="4"/>
         <v>0.38437494720124354</v>
       </c>
     </row>
-    <row r="14" spans="2:26">
+    <row r="14" spans="2:27">
       <c r="N14" s="16">
         <v>11</v>
       </c>
@@ -1704,33 +1783,36 @@
         <v>10979</v>
       </c>
       <c r="T14" s="13">
-        <v>192.3</v>
-      </c>
-      <c r="U14" s="17">
+        <v>315.5</v>
+      </c>
+      <c r="U14" s="40">
+        <v>289</v>
+      </c>
+      <c r="V14" s="25">
         <f t="shared" si="0"/>
-        <v>823.90000000000009</v>
-      </c>
-      <c r="V14">
+        <v>700.7</v>
+      </c>
+      <c r="W14">
         <f t="shared" si="1"/>
         <v>0.62199370202715998</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>0.62199370202715998</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <f t="shared" si="2"/>
-        <v>384.13000000000005</v>
-      </c>
-      <c r="Y14">
+        <v>384.13</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="3"/>
-        <v>0.18923440267663846</v>
-      </c>
-      <c r="Z14">
+        <v>0.3104703798464869</v>
+      </c>
+      <c r="AA14">
         <f t="shared" si="4"/>
         <v>0.37800629797284002</v>
       </c>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:27">
       <c r="N15" s="16">
         <v>12</v>
       </c>
@@ -1750,33 +1832,36 @@
         <v>11915</v>
       </c>
       <c r="T15" s="13">
-        <v>163.9</v>
-      </c>
-      <c r="U15" s="17">
+        <v>271.2</v>
+      </c>
+      <c r="U15" s="40">
+        <v>246.9</v>
+      </c>
+      <c r="V15" s="25">
         <f t="shared" si="0"/>
-        <v>715.79000000000008</v>
-      </c>
-      <c r="V15">
+        <v>608.49</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="1"/>
         <v>0.60397412724937183</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>0.60397412724937183</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <f t="shared" si="2"/>
         <v>348.38000000000011</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <f t="shared" si="3"/>
-        <v>0.18631563391649331</v>
-      </c>
-      <c r="Z15">
+        <v>0.30829042048903588</v>
+      </c>
+      <c r="AA15">
         <f t="shared" si="4"/>
         <v>0.39602587275062817</v>
       </c>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:27">
       <c r="N16" s="16">
         <v>13</v>
       </c>
@@ -1796,33 +1881,36 @@
         <v>12768</v>
       </c>
       <c r="T16" s="13">
-        <v>145.80000000000001</v>
-      </c>
-      <c r="U16" s="17">
+        <v>231.4</v>
+      </c>
+      <c r="U16" s="40">
+        <v>211.4</v>
+      </c>
+      <c r="V16" s="25">
         <f t="shared" si="0"/>
-        <v>617.5</v>
-      </c>
-      <c r="V16">
+        <v>531.9</v>
+      </c>
+      <c r="W16">
         <f t="shared" si="1"/>
         <v>0.63127210795231237</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>0.63127210795231237</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <f t="shared" si="2"/>
         <v>281.44999999999993</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <f t="shared" si="3"/>
-        <v>0.19101270797851438</v>
-      </c>
-      <c r="Z16">
+        <v>0.30315734311541992</v>
+      </c>
+      <c r="AA16">
         <f t="shared" si="4"/>
         <v>0.36872789204768763</v>
       </c>
     </row>
-    <row r="17" spans="14:26">
+    <row r="17" spans="14:27">
       <c r="N17" s="16">
         <v>14</v>
       </c>
@@ -1842,33 +1930,36 @@
         <v>13530</v>
       </c>
       <c r="T17" s="13">
-        <v>125.3</v>
-      </c>
-      <c r="U17" s="17">
+        <v>197.6</v>
+      </c>
+      <c r="U17" s="40">
+        <v>183</v>
+      </c>
+      <c r="V17" s="25">
         <f t="shared" si="0"/>
-        <v>538.20000000000005</v>
-      </c>
-      <c r="V17">
+        <v>465.9</v>
+      </c>
+      <c r="W17">
         <f t="shared" si="1"/>
         <v>0.62449133383571975</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>0.62449133383571975</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <f t="shared" si="2"/>
-        <v>249.14999999999995</v>
-      </c>
-      <c r="Y17">
+        <v>249.14999999999998</v>
+      </c>
+      <c r="Z17">
         <f t="shared" si="3"/>
-        <v>0.18884702336096457</v>
-      </c>
-      <c r="Z17">
+        <v>0.29781461944235116</v>
+      </c>
+      <c r="AA17">
         <f t="shared" si="4"/>
         <v>0.37550866616428025</v>
       </c>
     </row>
-    <row r="18" spans="14:26">
+    <row r="18" spans="14:27">
       <c r="N18" s="16">
         <v>15</v>
       </c>
@@ -1888,33 +1979,36 @@
         <v>14227</v>
       </c>
       <c r="T18" s="13">
-        <v>108</v>
-      </c>
-      <c r="U18" s="17">
+        <v>172.3</v>
+      </c>
+      <c r="U18" s="40">
+        <v>163.1</v>
+      </c>
+      <c r="V18" s="25">
         <f t="shared" si="0"/>
-        <v>480.03999999999996</v>
-      </c>
-      <c r="V18">
+        <v>415.73999999999995</v>
+      </c>
+      <c r="W18">
         <f t="shared" si="1"/>
         <v>0.61506019998639549</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>0.61506019998639549</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <f t="shared" si="2"/>
-        <v>226.35999999999999</v>
-      </c>
-      <c r="Y18">
+        <v>226.35999999999996</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="3"/>
-        <v>0.18366097544384738</v>
-      </c>
-      <c r="Z18">
+        <v>0.29300727841643431</v>
+      </c>
+      <c r="AA18">
         <f t="shared" si="4"/>
         <v>0.38493980001360451</v>
       </c>
     </row>
-    <row r="19" spans="14:26">
+    <row r="19" spans="14:27">
       <c r="N19" s="16">
         <v>16</v>
       </c>
@@ -1934,33 +2028,36 @@
         <v>14990</v>
       </c>
       <c r="T19" s="13">
-        <v>93.7</v>
-      </c>
-      <c r="U19" s="17">
+        <v>152.69999999999999</v>
+      </c>
+      <c r="U19" s="40">
+        <v>144.6</v>
+      </c>
+      <c r="V19" s="25">
         <f t="shared" si="0"/>
-        <v>442.59</v>
-      </c>
-      <c r="V19">
+        <v>383.59</v>
+      </c>
+      <c r="W19">
         <f t="shared" si="1"/>
         <v>0.63051707098771193</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>0.63051707098771193</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <f t="shared" si="2"/>
-        <v>198.14999999999995</v>
-      </c>
-      <c r="Y19">
+        <v>198.14999999999998</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="3"/>
-        <v>0.17471890208655766</v>
-      </c>
-      <c r="Z19">
+        <v>0.28473400585504111</v>
+      </c>
+      <c r="AA19">
         <f t="shared" si="4"/>
         <v>0.36948292901228807</v>
       </c>
     </row>
-    <row r="20" spans="14:26">
+    <row r="20" spans="14:27">
       <c r="N20" s="16">
         <v>17</v>
       </c>
@@ -1980,33 +2077,36 @@
         <v>15671</v>
       </c>
       <c r="T20" s="13">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="U20" s="17">
+        <v>136.19999999999999</v>
+      </c>
+      <c r="U20" s="40">
+        <v>126.7</v>
+      </c>
+      <c r="V20" s="25">
         <f t="shared" si="0"/>
-        <v>391.39</v>
-      </c>
-      <c r="V20">
+        <v>337.09000000000003</v>
+      </c>
+      <c r="W20">
         <f t="shared" si="1"/>
         <v>0.6580532020537091</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>0.6580532020537091</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <f t="shared" si="2"/>
         <v>161.84000000000003</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <f t="shared" si="3"/>
-        <v>0.17304401107143613</v>
-      </c>
-      <c r="Z20">
+        <v>0.28777282427264467</v>
+      </c>
+      <c r="AA20">
         <f t="shared" si="4"/>
         <v>0.3419467979462909</v>
       </c>
     </row>
-    <row r="21" spans="14:26">
+    <row r="21" spans="14:27">
       <c r="N21" s="16">
         <v>18</v>
       </c>
@@ -2026,33 +2126,36 @@
         <v>16493</v>
       </c>
       <c r="T21" s="13">
-        <v>69.8</v>
-      </c>
-      <c r="U21" s="17">
+        <v>119.4</v>
+      </c>
+      <c r="U21" s="40">
+        <v>110.2</v>
+      </c>
+      <c r="V21" s="25">
         <f t="shared" si="0"/>
-        <v>352.17</v>
-      </c>
-      <c r="V21">
+        <v>302.57000000000005</v>
+      </c>
+      <c r="W21">
         <f t="shared" si="1"/>
         <v>0.63997440576344289</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>0.63997440576344289</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <f t="shared" si="2"/>
         <v>151.92000000000002</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <f t="shared" si="3"/>
-        <v>0.16541460293385785</v>
-      </c>
-      <c r="Z21">
+        <v>0.28295850415906343</v>
+      </c>
+      <c r="AA21">
         <f t="shared" si="4"/>
         <v>0.36002559423655711</v>
       </c>
     </row>
-    <row r="22" spans="14:26">
+    <row r="22" spans="14:27">
       <c r="N22" s="16">
         <v>19</v>
       </c>
@@ -2072,33 +2175,36 @@
         <v>17256</v>
       </c>
       <c r="T22" s="13">
-        <v>59.7</v>
-      </c>
-      <c r="U22" s="17">
+        <v>103.8</v>
+      </c>
+      <c r="U22" s="40">
+        <v>98.7</v>
+      </c>
+      <c r="V22" s="25">
         <f t="shared" si="0"/>
-        <v>312.83</v>
-      </c>
-      <c r="V22">
+        <v>268.72999999999996</v>
+      </c>
+      <c r="W22">
         <f t="shared" si="1"/>
         <v>0.64341126889109601</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>0.64341126889109601</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <f t="shared" si="2"/>
-        <v>132.84</v>
-      </c>
-      <c r="Y22">
+        <v>132.83999999999997</v>
+      </c>
+      <c r="Z22">
         <f t="shared" si="3"/>
-        <v>0.16025554988859961</v>
-      </c>
-      <c r="Z22">
+        <v>0.27863527769575608</v>
+      </c>
+      <c r="AA22">
         <f t="shared" si="4"/>
         <v>0.35658873110890399</v>
       </c>
     </row>
-    <row r="23" spans="14:26">
+    <row r="23" spans="14:27">
       <c r="N23" s="16">
         <v>20</v>
       </c>
@@ -2118,33 +2224,36 @@
         <v>18097</v>
       </c>
       <c r="T23" s="13">
-        <v>48.9</v>
-      </c>
-      <c r="U23" s="17">
+        <v>89.2</v>
+      </c>
+      <c r="U23" s="40">
+        <v>85.3</v>
+      </c>
+      <c r="V23" s="25">
         <f t="shared" si="0"/>
-        <v>289.69</v>
-      </c>
-      <c r="V23">
+        <v>249.39</v>
+      </c>
+      <c r="W23">
         <f t="shared" si="1"/>
         <v>0.65406538881833498</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>0.65406538881833498</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <f t="shared" si="2"/>
-        <v>117.12999999999995</v>
-      </c>
-      <c r="Y23">
+        <v>117.12999999999997</v>
+      </c>
+      <c r="Z23">
         <f t="shared" si="3"/>
-        <v>0.14442245783986532</v>
-      </c>
-      <c r="Z23">
+        <v>0.26344546501668686</v>
+      </c>
+      <c r="AA23">
         <f t="shared" si="4"/>
         <v>0.34593461118166502</v>
       </c>
     </row>
-    <row r="24" spans="14:26">
+    <row r="24" spans="14:27">
       <c r="N24" s="16">
         <v>21</v>
       </c>
@@ -2164,33 +2273,36 @@
         <v>18744</v>
       </c>
       <c r="T24" s="13">
-        <v>43.7</v>
-      </c>
-      <c r="U24" s="17">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="U24" s="40">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="V24" s="25">
         <f t="shared" si="0"/>
-        <v>254.18</v>
-      </c>
-      <c r="V24">
+        <v>218.48</v>
+      </c>
+      <c r="W24">
         <f t="shared" si="1"/>
         <v>0.66849066738283869</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>0.66849066738283869</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <f t="shared" si="2"/>
-        <v>98.750000000000014</v>
-      </c>
-      <c r="Y24">
+        <v>98.75</v>
+      </c>
+      <c r="Z24">
         <f t="shared" si="3"/>
-        <v>0.14670337048475898</v>
-      </c>
-      <c r="Z24">
+        <v>0.26655028870686187</v>
+      </c>
+      <c r="AA24">
         <f t="shared" si="4"/>
         <v>0.33150933261716131</v>
       </c>
     </row>
-    <row r="25" spans="14:26">
+    <row r="25" spans="14:27">
       <c r="N25" s="16">
         <v>22</v>
       </c>
@@ -2210,33 +2322,36 @@
         <v>19447</v>
       </c>
       <c r="T25" s="13">
-        <v>36.6</v>
-      </c>
-      <c r="U25" s="17">
+        <v>68.7</v>
+      </c>
+      <c r="U25" s="40">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="V25" s="25">
         <f t="shared" si="0"/>
-        <v>231.45000000000002</v>
-      </c>
-      <c r="V25">
+        <v>199.35000000000002</v>
+      </c>
+      <c r="W25">
         <f t="shared" si="1"/>
         <v>0.66592053721320643</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>0.66592053721320643</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <f t="shared" si="2"/>
-        <v>89.550000000000026</v>
-      </c>
-      <c r="Y25">
+        <v>89.550000000000011</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="3"/>
-        <v>0.13654168998321209</v>
-      </c>
-      <c r="Z25">
+        <v>0.25629546726357022</v>
+      </c>
+      <c r="AA25">
         <f t="shared" si="4"/>
         <v>0.33407946278679357</v>
       </c>
     </row>
-    <row r="26" spans="14:26">
+    <row r="26" spans="14:27">
       <c r="N26" s="16">
         <v>23</v>
       </c>
@@ -2256,33 +2371,36 @@
         <v>20130</v>
       </c>
       <c r="T26" s="13">
-        <v>31.4</v>
-      </c>
-      <c r="U26" s="17">
+        <v>58.8</v>
+      </c>
+      <c r="U26" s="40">
+        <v>53.7</v>
+      </c>
+      <c r="V26" s="25">
         <f t="shared" si="0"/>
-        <v>197.71</v>
-      </c>
-      <c r="V26">
+        <v>170.31</v>
+      </c>
+      <c r="W26">
         <f t="shared" si="1"/>
         <v>0.67325738728121853</v>
       </c>
-      <c r="W26">
+      <c r="X26">
         <v>0.67325738728121853</v>
       </c>
-      <c r="X26">
+      <c r="Y26">
         <f t="shared" si="2"/>
-        <v>74.860000000000028</v>
-      </c>
-      <c r="Y26">
+        <v>74.860000000000014</v>
+      </c>
+      <c r="Z26">
         <f t="shared" si="3"/>
-        <v>0.13705207105757058</v>
-      </c>
-      <c r="Z26">
+        <v>0.25664527956003663</v>
+      </c>
+      <c r="AA26">
         <f t="shared" si="4"/>
         <v>0.32674261271878147</v>
       </c>
     </row>
-    <row r="27" spans="14:26">
+    <row r="27" spans="14:27">
       <c r="N27" s="16">
         <v>24</v>
       </c>
@@ -2302,33 +2420,36 @@
         <v>21097</v>
       </c>
       <c r="T27" s="13">
-        <v>24.3</v>
-      </c>
-      <c r="U27" s="17">
+        <v>50</v>
+      </c>
+      <c r="U27" s="40">
+        <v>47.1</v>
+      </c>
+      <c r="V27" s="25">
         <f t="shared" si="0"/>
-        <v>177.44</v>
-      </c>
-      <c r="V27">
+        <v>151.74</v>
+      </c>
+      <c r="W27">
         <f t="shared" si="1"/>
         <v>0.68023198175869926</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>0.68023198175869926</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <f t="shared" si="2"/>
         <v>64.510000000000019</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <f t="shared" si="3"/>
-        <v>0.1204520670169525</v>
-      </c>
-      <c r="Z27">
+        <v>0.24784375929414096</v>
+      </c>
+      <c r="AA27">
         <f t="shared" si="4"/>
         <v>0.31976801824130074</v>
       </c>
     </row>
-    <row r="28" spans="14:26">
+    <row r="28" spans="14:27">
       <c r="N28" s="16">
         <v>25</v>
       </c>
@@ -2348,33 +2469,36 @@
         <v>21849</v>
       </c>
       <c r="T28" s="13">
-        <v>18.3</v>
-      </c>
-      <c r="U28" s="17">
+        <v>42.9</v>
+      </c>
+      <c r="U28" s="40">
+        <v>38.6</v>
+      </c>
+      <c r="V28" s="25">
         <f t="shared" si="0"/>
-        <v>157.91999999999999</v>
-      </c>
-      <c r="V28">
+        <v>133.32</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="1"/>
         <v>0.69027352173419587</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>0.69027352173419587</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <f t="shared" si="2"/>
-        <v>54.580000000000005</v>
-      </c>
-      <c r="Y28">
+        <v>54.58</v>
+      </c>
+      <c r="Z28">
         <f t="shared" si="3"/>
-        <v>0.1038474633980252</v>
-      </c>
-      <c r="Z28">
+        <v>0.24344569288389512</v>
+      </c>
+      <c r="AA28">
         <f t="shared" si="4"/>
         <v>0.30972647826580413</v>
       </c>
     </row>
-    <row r="29" spans="14:26">
+    <row r="29" spans="14:27">
       <c r="N29" s="16">
         <v>26</v>
       </c>
@@ -2394,33 +2518,36 @@
         <v>22975</v>
       </c>
       <c r="T29" s="13">
-        <v>13</v>
-      </c>
-      <c r="U29" s="17">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="U29" s="40">
+        <v>30.5</v>
+      </c>
+      <c r="V29" s="25">
         <f t="shared" si="0"/>
-        <v>134.13</v>
-      </c>
-      <c r="V29">
+        <v>113.42999999999999</v>
+      </c>
+      <c r="W29">
         <f t="shared" si="1"/>
         <v>0.66546591449738324</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>0.66546591449738324</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <f t="shared" si="2"/>
-        <v>49.220000000000006</v>
-      </c>
-      <c r="Y29">
+        <v>49.22</v>
+      </c>
+      <c r="Z29">
         <f t="shared" si="3"/>
-        <v>8.8357235098212472E-2</v>
-      </c>
-      <c r="Z29">
+        <v>0.22904914021613543</v>
+      </c>
+      <c r="AA29">
         <f t="shared" si="4"/>
         <v>0.33453408550261676</v>
       </c>
     </row>
-    <row r="30" spans="14:26">
+    <row r="30" spans="14:27">
       <c r="N30" s="16">
         <v>27</v>
       </c>
@@ -2440,33 +2567,36 @@
         <v>23848</v>
       </c>
       <c r="T30" s="13">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="U30" s="17">
+        <v>27.4</v>
+      </c>
+      <c r="U30" s="40">
+        <v>24</v>
+      </c>
+      <c r="V30" s="25">
         <f t="shared" si="0"/>
-        <v>121.96999999999998</v>
-      </c>
-      <c r="V30">
+        <v>103.26999999999998</v>
+      </c>
+      <c r="W30">
         <f t="shared" si="1"/>
         <v>0.69220172954771575</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>0.69220172954771575</v>
       </c>
-      <c r="X30">
+      <c r="Y30">
         <f t="shared" si="2"/>
-        <v>40.219999999999978</v>
-      </c>
-      <c r="Y30">
+        <v>40.219999999999985</v>
+      </c>
+      <c r="Z30">
         <f t="shared" si="3"/>
-        <v>6.6579934185352421E-2</v>
-      </c>
-      <c r="Z30">
+        <v>0.20968852835386853</v>
+      </c>
+      <c r="AA30">
         <f t="shared" si="4"/>
         <v>0.30779827045228425</v>
       </c>
     </row>
-    <row r="31" spans="14:26">
+    <row r="31" spans="14:27">
       <c r="N31" s="16">
         <v>28</v>
       </c>
@@ -2486,33 +2616,36 @@
         <v>24739</v>
       </c>
       <c r="T31" s="13">
-        <v>6.9</v>
-      </c>
-      <c r="U31" s="17">
+        <v>22</v>
+      </c>
+      <c r="U31" s="40">
+        <v>20</v>
+      </c>
+      <c r="V31" s="25">
         <f t="shared" si="0"/>
-        <v>104.14</v>
-      </c>
-      <c r="V31">
+        <v>89.04</v>
+      </c>
+      <c r="W31">
         <f t="shared" si="1"/>
         <v>0.70307997118155607</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>0.70307997118155607</v>
       </c>
-      <c r="X31">
+      <c r="Y31">
         <f t="shared" si="2"/>
         <v>32.970000000000013</v>
       </c>
-      <c r="Y31">
+      <c r="Z31">
         <f t="shared" si="3"/>
-        <v>6.2139769452449568E-2</v>
-      </c>
-      <c r="Z31">
+        <v>0.19812680115273773</v>
+      </c>
+      <c r="AA31">
         <f t="shared" si="4"/>
         <v>0.29692002881844393</v>
       </c>
     </row>
-    <row r="32" spans="14:26">
+    <row r="32" spans="14:27">
       <c r="N32" s="16">
         <v>29</v>
       </c>
@@ -2532,33 +2665,36 @@
         <v>25760</v>
       </c>
       <c r="T32" s="13">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="U32" s="17">
+        <v>18.2</v>
+      </c>
+      <c r="U32" s="40">
+        <v>15.1</v>
+      </c>
+      <c r="V32" s="25">
         <f t="shared" si="0"/>
-        <v>89.64</v>
-      </c>
-      <c r="V32">
+        <v>73.64</v>
+      </c>
+      <c r="W32">
         <f t="shared" si="1"/>
         <v>0.68967770034843212</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>0.68967770034843212</v>
       </c>
-      <c r="X32">
+      <c r="Y32">
         <f t="shared" si="2"/>
-        <v>28.499999999999996</v>
-      </c>
-      <c r="Y32">
+        <v>28.5</v>
+      </c>
+      <c r="Z32">
         <f t="shared" si="3"/>
-        <v>2.3954703832752614E-2</v>
-      </c>
-      <c r="Z32">
+        <v>0.19817073170731705</v>
+      </c>
+      <c r="AA32">
         <f t="shared" si="4"/>
         <v>0.31032229965156788</v>
       </c>
     </row>
-    <row r="33" spans="14:26">
+    <row r="33" spans="14:27">
       <c r="N33" s="16">
         <v>30</v>
       </c>
@@ -2578,33 +2714,36 @@
         <v>26616</v>
       </c>
       <c r="T33" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="U33" s="17">
+        <v>12.5</v>
+      </c>
+      <c r="U33" s="40">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="V33" s="25">
         <f t="shared" si="0"/>
-        <v>78.150000000000006</v>
-      </c>
-      <c r="V33">
+        <v>65.95</v>
+      </c>
+      <c r="W33">
         <f t="shared" si="1"/>
         <v>0.68540471637985978</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>0.68540471637985978</v>
       </c>
-      <c r="X33">
+      <c r="Y33">
         <f t="shared" si="2"/>
         <v>24.68</v>
       </c>
-      <c r="Y33">
+      <c r="Z33">
         <f t="shared" si="3"/>
-        <v>3.8240917782026767E-3</v>
-      </c>
-      <c r="Z33">
+        <v>0.15933715742511154</v>
+      </c>
+      <c r="AA33">
         <f t="shared" si="4"/>
         <v>0.31459528362014022</v>
       </c>
     </row>
-    <row r="34" spans="14:26">
+    <row r="34" spans="14:27">
       <c r="N34" s="16">
         <v>31</v>
       </c>
@@ -2624,79 +2763,85 @@
         <v>27339</v>
       </c>
       <c r="T34" s="13">
-        <v>1</v>
-      </c>
-      <c r="U34" s="17">
+        <v>7</v>
+      </c>
+      <c r="U34" s="40">
+        <v>9.5</v>
+      </c>
+      <c r="V34" s="25">
         <f t="shared" si="0"/>
-        <v>62.65</v>
-      </c>
-      <c r="V34">
+        <v>56.65</v>
+      </c>
+      <c r="W34">
         <f t="shared" si="1"/>
         <v>0.71563236449332279</v>
       </c>
-      <c r="W34">
+      <c r="X34">
         <v>0.71563236449332279</v>
       </c>
-      <c r="X34">
+      <c r="Y34">
         <f t="shared" si="2"/>
-        <v>18.100000000000005</v>
-      </c>
-      <c r="Y34">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="Z34">
         <f t="shared" si="3"/>
-        <v>1.5710919088766692E-2</v>
-      </c>
-      <c r="Z34">
+        <v>0.10997643362136686</v>
+      </c>
+      <c r="AA34">
         <f t="shared" si="4"/>
         <v>0.28436763550667721</v>
       </c>
     </row>
-    <row r="35" spans="14:26" ht="15.75" thickBot="1">
-      <c r="N35" s="18">
+    <row r="35" spans="14:27" ht="15.75" thickBot="1">
+      <c r="N35" s="17">
         <v>32</v>
       </c>
-      <c r="O35" s="19">
+      <c r="O35" s="18">
         <v>54.69</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="18">
         <v>39.700000000000003</v>
       </c>
-      <c r="Q35" s="20">
+      <c r="Q35" s="19">
         <v>0.95740000000000003</v>
       </c>
-      <c r="R35" s="21">
+      <c r="R35" s="20">
         <v>99.052616666666665</v>
       </c>
-      <c r="S35" s="19">
+      <c r="S35" s="18">
         <v>27387</v>
       </c>
-      <c r="T35" s="19">
-        <v>2.5</v>
-      </c>
-      <c r="U35" s="22">
+      <c r="T35" s="18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U35" s="41">
+        <v>2.8</v>
+      </c>
+      <c r="V35" s="25">
         <f t="shared" si="0"/>
-        <v>52.19</v>
-      </c>
-      <c r="V35">
+        <v>49.79</v>
+      </c>
+      <c r="W35">
         <f t="shared" si="1"/>
         <v>0.72590967270067663</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>0.72590967270067663</v>
       </c>
-      <c r="X35">
+      <c r="Y35">
         <f t="shared" si="2"/>
         <v>14.989999999999995</v>
       </c>
-      <c r="Y35">
+      <c r="Z35">
         <f t="shared" si="3"/>
-        <v>4.5712196013896512E-2</v>
-      </c>
-      <c r="Z35">
+        <v>8.959590418723716E-2</v>
+      </c>
+      <c r="AA35">
         <f t="shared" si="4"/>
         <v>0.27409032729932337</v>
       </c>
     </row>
-    <row r="36" spans="14:26">
+    <row r="36" spans="14:27">
       <c r="P36" t="s">
         <v>10</v>
       </c>
@@ -2705,7 +2850,7 @@
         <v>0.94159999999999999</v>
       </c>
     </row>
-    <row r="37" spans="14:26">
+    <row r="37" spans="14:27">
       <c r="P37" t="s">
         <v>11</v>
       </c>
@@ -2714,7 +2859,7 @@
         <v>0.96040000000000003</v>
       </c>
     </row>
-    <row r="38" spans="14:26">
+    <row r="38" spans="14:27">
       <c r="P38" t="s">
         <v>12</v>
       </c>
@@ -2723,7 +2868,7 @@
         <v>1.8800000000000039E-2</v>
       </c>
     </row>
-    <row r="39" spans="14:26">
+    <row r="39" spans="14:27">
       <c r="P39" t="s">
         <v>13</v>
       </c>
@@ -2732,7 +2877,7 @@
         <v>0.95335000000000003</v>
       </c>
     </row>
-    <row r="40" spans="14:26">
+    <row r="40" spans="14:27">
       <c r="P40" t="s">
         <v>14</v>
       </c>
@@ -2745,7 +2890,7 @@
         <v>1.232495935385749</v>
       </c>
     </row>
-    <row r="41" spans="14:26">
+    <row r="41" spans="14:27">
       <c r="P41" t="s">
         <v>15</v>
       </c>
@@ -2755,20 +2900,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B3:B4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="U2:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>